<commit_message>
Update Products.xlsx with new product data and configurations.
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Howard Lee\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C1310E-BEB8-4DD9-9D38-C91408EC9B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EBAA21-4530-4B7F-8A25-323359AD13FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1E993779-62B1-4F53-9190-FE1F7B4CDCE0}"/>
+    <workbookView xWindow="15090" yWindow="6900" windowWidth="24300" windowHeight="15690" xr2:uid="{1E993779-62B1-4F53-9190-FE1F7B4CDCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>SKU</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>2.4 X 3.6 INCH</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>girl1</t>
+  </si>
+  <si>
+    <t>boy1</t>
+  </si>
+  <si>
+    <t>boy2</t>
   </si>
 </sst>
 </file>
@@ -555,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BCE57D-9218-428D-AA51-4B87D71DD09E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -567,9 +579,10 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -591,8 +604,11 @@
       <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -614,8 +630,11 @@
       <c r="G2" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -637,8 +656,11 @@
       <c r="G3" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -660,8 +682,11 @@
       <c r="G4" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -684,7 +709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -707,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -730,7 +755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -753,7 +778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -776,7 +801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -799,7 +824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -822,7 +847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -845,7 +870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -868,7 +893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -891,7 +916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -914,7 +939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>7</v>
       </c>

</xml_diff>